<commit_message>
Updated wooden panels measurements
</commit_message>
<xml_diff>
--- a/hardware/control-panel/parameters.xlsx
+++ b/hardware/control-panel/parameters.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Dokument\Projekt\Elita\Electrical system\Highside-Powerdistribution\hardware\control-panel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskar\Dropbox\Dokument\Projekt\Elita\Electrical system\Highside-Powerdistribution\hardware\control-panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70233A60-01AC-412B-9AB4-BBD1E0170D21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A85D489-74D5-41BA-9C98-6B4AA21DAF5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>mm</t>
   </si>
@@ -130,6 +138,18 @@
   </si>
   <si>
     <t>l_fastener_button</t>
+  </si>
+  <si>
+    <t>w_infosign</t>
+  </si>
+  <si>
+    <t>l_infosign</t>
+  </si>
+  <si>
+    <t>w_hidden_panel</t>
+  </si>
+  <si>
+    <t>Part that is hidden by another piece</t>
   </si>
 </sst>
 </file>
@@ -447,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -488,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -530,7 +550,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -544,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -673,7 +693,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -684,7 +704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -693,6 +713,42 @@
       </c>
       <c r="C18" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>180</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>